<commit_message>
Streamlined ExcelSheet.java and improved test output
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\MC\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C1DC9D46-63A2-42C3-A16B-A636793D7AA8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B8C356D9-4D7E-4931-AEC4-60F06B02E828}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{76F07B30-AB82-42C6-9B03-FAE294972B07}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Sentence Text</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Expected Length of Longest Word</t>
   </si>
   <si>
-    <t>Goose</t>
-  </si>
-  <si>
     <t>Expected Longest Word(s)</t>
   </si>
   <si>
@@ -67,6 +64,30 @@
   </si>
   <si>
     <t>properlyhyphenated</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>MotherGoose</t>
+  </si>
+  <si>
+    <t>one-word sentence</t>
+  </si>
+  <si>
+    <t>longest word is followed by punctuation</t>
+  </si>
+  <si>
+    <t>duplicate longest words</t>
+  </si>
+  <si>
+    <t>single longest word</t>
+  </si>
+  <si>
+    <t>longest word is apostrophized</t>
+  </si>
+  <si>
+    <t>longest word is hyphenated</t>
   </si>
 </sst>
 </file>
@@ -445,95 +466,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61FD5F1-8515-4686-9F45-59426DD71E81}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="64" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="C3" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="C5" s="1">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="1">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="1">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="1">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Only strip punctuation if it occurs at the end of a word
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\MC\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B8C356D9-4D7E-4931-AEC4-60F06B02E828}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100800_{8CECB0F4-6004-4F9B-9CB4-8B92141F3B34}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{76F07B30-AB82-42C6-9B03-FAE294972B07}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="7005" xr2:uid="{76F07B30-AB82-42C6-9B03-FAE294972B07}"/>
   </bookViews>
   <sheets>
     <sheet name="WordLength" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,15 +53,9 @@
     <t>Shouldn't the longest word in this example have a length of nine?</t>
   </si>
   <si>
-    <t>Shouldnt</t>
-  </si>
-  <si>
     <t>Shouldn't the longest word in this example have a properly-hyphenated length of nineteen?</t>
   </si>
   <si>
-    <t>properlyhyphenated</t>
-  </si>
-  <si>
     <t>Test Description</t>
   </si>
   <si>
@@ -88,6 +78,12 @@
   </si>
   <si>
     <t>longest word is hyphenated</t>
+  </si>
+  <si>
+    <t>Shouldn't</t>
+  </si>
+  <si>
+    <t>properly-hyphenated</t>
   </si>
 </sst>
 </file>
@@ -468,9 +464,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61FD5F1-8515-4686-9F45-59426DD71E81}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +479,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -497,21 +493,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -525,7 +521,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -539,7 +535,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -553,30 +549,30 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhanced documentation and added test case for ends with '
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100800_{8CECB0F4-6004-4F9B-9CB4-8B92141F3B34}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\MC\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{337B13B0-11CF-4A92-96E3-3440E1D903FA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="7005" xr2:uid="{76F07B30-AB82-42C6-9B03-FAE294972B07}"/>
   </bookViews>
@@ -11,7 +16,6 @@
     <sheet name="WordLength" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Sentence Text</t>
   </si>
@@ -84,6 +88,15 @@
   </si>
   <si>
     <t>properly-hyphenated</t>
+  </si>
+  <si>
+    <t>longest word ends with apostrophe</t>
+  </si>
+  <si>
+    <t>The big words' end.</t>
+  </si>
+  <si>
+    <t>words'</t>
   </si>
 </sst>
 </file>
@@ -462,11 +475,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61FD5F1-8515-4686-9F45-59426DD71E81}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,6 +588,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>